<commit_message>
migrate to chip db + lineup gui
</commit_message>
<xml_diff>
--- a/lineups/FS - TalynM.Tx BoardFile FW.xlsx
+++ b/lineups/FS - TalynM.Tx BoardFile FW.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>Temp</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>note</t>
-  </si>
-  <si>
-    <t>Note!</t>
   </si>
 </sst>
 </file>
@@ -410,7 +407,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,13 +473,13 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2">
-        <v>-40</v>
+        <v>-30</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -494,25 +491,25 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -524,21 +521,21 @@
         <v>1</v>
       </c>
       <c r="Q2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3">
-        <v>-40</v>
+        <v>-30</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -550,25 +547,25 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -580,15 +577,15 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4">
-        <v>-40</v>
+        <v>-30</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -606,25 +603,25 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -636,15 +633,15 @@
         <v>1</v>
       </c>
       <c r="Q4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5">
-        <v>-40</v>
+        <v>-30</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -662,25 +659,25 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -692,77 +689,77 @@
         <v>1</v>
       </c>
       <c r="Q5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6">
-        <v>-40</v>
+        <v>-30</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
         <v>3</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>3</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
       <c r="R6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7">
-        <v>-40</v>
+        <v>-30</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -774,51 +771,51 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
+        <v>6</v>
+      </c>
+      <c r="M7">
+        <v>2</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
         <v>5</v>
       </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
       <c r="R7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8">
-        <v>-20</v>
+        <v>-30</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -830,25 +827,25 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -860,21 +857,21 @@
         <v>1</v>
       </c>
       <c r="Q8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9">
-        <v>-20</v>
+        <v>-30</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -886,25 +883,25 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -916,21 +913,21 @@
         <v>1</v>
       </c>
       <c r="Q9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:18">
       <c r="A10">
-        <v>-20</v>
+        <v>-30</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -942,25 +939,25 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -972,21 +969,21 @@
         <v>1</v>
       </c>
       <c r="Q10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:18">
       <c r="A11">
-        <v>-20</v>
+        <v>-30</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -998,25 +995,25 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -1028,122 +1025,794 @@
         <v>1</v>
       </c>
       <c r="Q11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="A12">
-        <v>-20</v>
+        <v>-30</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>6</v>
+      </c>
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
         <v>3</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>3</v>
-      </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-      <c r="O12">
-        <v>1</v>
-      </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
-      <c r="Q12">
-        <v>1</v>
-      </c>
       <c r="R12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="A13">
-        <v>-20</v>
+        <v>-30</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>6</v>
+      </c>
+      <c r="M13">
+        <v>2</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>5</v>
+      </c>
+      <c r="R13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14">
+        <v>-10</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>4</v>
+      </c>
+      <c r="M14">
+        <v>2</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15">
+        <v>-10</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>4</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
         <v>3</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
+      <c r="R15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16">
+        <v>-10</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>4</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
         <v>5</v>
       </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
-      <c r="O13">
-        <v>1</v>
-      </c>
-      <c r="P13">
-        <v>1</v>
-      </c>
-      <c r="Q13">
-        <v>1</v>
-      </c>
-      <c r="R13" t="s">
-        <v>18</v>
+      <c r="R16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17">
+        <v>-10</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>6</v>
+      </c>
+      <c r="M17">
+        <v>2</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18">
+        <v>-10</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>6</v>
+      </c>
+      <c r="M18">
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>3</v>
+      </c>
+      <c r="R18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19">
+        <v>-10</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>6</v>
+      </c>
+      <c r="M19">
+        <v>2</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>5</v>
+      </c>
+      <c r="R19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20">
+        <v>-10</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>4</v>
+      </c>
+      <c r="M20">
+        <v>2</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21">
+        <v>-10</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>4</v>
+      </c>
+      <c r="M21">
+        <v>2</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>3</v>
+      </c>
+      <c r="R21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22">
+        <v>-10</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>4</v>
+      </c>
+      <c r="M22">
+        <v>2</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>5</v>
+      </c>
+      <c r="R22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23">
+        <v>-10</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>6</v>
+      </c>
+      <c r="M23">
+        <v>2</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24">
+        <v>-10</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>6</v>
+      </c>
+      <c r="M24">
+        <v>2</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>3</v>
+      </c>
+      <c r="R24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25">
+        <v>-10</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>6</v>
+      </c>
+      <c r="M25">
+        <v>2</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>5</v>
+      </c>
+      <c r="R25" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>